<commit_message>
Add new integration test
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/new_labels.xlsx
+++ b/tests/integration_test_files/new_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4EE837-E468-0340-AA33-F659D00F5540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6346BD17-ACEC-E842-A798-DC16958DEC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38160" yWindow="4280" windowWidth="33600" windowHeight="19480" firstSheet="3" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="66180" yWindow="7680" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="559">
   <si>
     <t>Epoch</t>
   </si>
@@ -147,12 +147,6 @@
   </si>
   <si>
     <t>organisationIdentifier</t>
-  </si>
-  <si>
-    <t>organisationName</t>
-  </si>
-  <si>
-    <t>organisationType</t>
   </si>
   <si>
     <t>studyIdentifier</t>
@@ -1756,6 +1750,12 @@
   </si>
   <si>
     <t>Drug A</t>
+  </si>
+  <si>
+    <t>CT.gov</t>
+  </si>
+  <si>
+    <t>ACME</t>
   </si>
 </sst>
 </file>
@@ -2260,7 +2260,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -2302,7 +2302,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -2313,10 +2313,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -2365,42 +2365,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="E9" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="F9" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="G9" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="H9" s="21" t="s">
         <v>150</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>156</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -2410,33 +2410,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G11" s="15">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2543,205 +2543,205 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>97</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2954,90 +2954,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
         <v>134</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>138</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
         <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
         <v>171</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>172</v>
       </c>
-      <c r="C5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" t="s">
         <v>173</v>
-      </c>
-      <c r="E5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -3066,65 +3066,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" t="s">
         <v>191</v>
-      </c>
-      <c r="B2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>195</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="G3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3157,137 +3157,137 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>214</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3314,104 +3314,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>240</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>235</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3438,16 +3438,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
@@ -3456,1212 +3456,1212 @@
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>554</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="10" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B44" s="26"/>
       <c r="C44" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B52" s="26"/>
       <c r="C52" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B55" s="26"/>
       <c r="C55" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B56" s="26"/>
       <c r="C56" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B57" s="26"/>
       <c r="C57" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B58" s="26"/>
       <c r="C58" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B59" s="26"/>
       <c r="C59" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B60" s="26"/>
       <c r="C60" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B61" s="26"/>
       <c r="C61" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B62" s="26"/>
       <c r="C62" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B63" s="26"/>
       <c r="C63" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B64" s="26"/>
       <c r="C64" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B65" s="26"/>
       <c r="C65" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B66" s="26"/>
       <c r="C66" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B67" s="26"/>
       <c r="C67" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B68" s="26"/>
       <c r="C68" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B69" s="26"/>
       <c r="C69" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B70" s="26"/>
       <c r="C70" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B71" s="26"/>
       <c r="C71" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B72" s="26"/>
       <c r="C72" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B73" s="26"/>
       <c r="C73" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B74" s="26"/>
       <c r="C74" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B75" s="26"/>
       <c r="C75" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B76" s="26"/>
       <c r="C76" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B77" s="26"/>
       <c r="C77" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B78" s="26"/>
       <c r="C78" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B79" s="26"/>
       <c r="C79" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B80" s="26"/>
       <c r="C80" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B82" s="26"/>
       <c r="C82" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B83" s="26"/>
       <c r="C83" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B84" s="26"/>
       <c r="C84" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B85" s="26"/>
       <c r="C85" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B86" s="26"/>
       <c r="C86" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B87" s="26"/>
       <c r="C87" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B88" s="26"/>
       <c r="C88" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B89" s="26"/>
       <c r="C89" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B90" s="26"/>
       <c r="C90" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B92" s="26"/>
       <c r="C92" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B93" s="26"/>
       <c r="C93" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B94" s="26"/>
       <c r="C94" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B95" s="26"/>
       <c r="C95" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B96" s="26"/>
       <c r="C96" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B97" s="26"/>
       <c r="C97" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B98" s="26"/>
       <c r="C98" s="10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B99" s="26"/>
       <c r="C99" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B100" s="26"/>
       <c r="C100" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B101" s="26"/>
       <c r="C101" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B102" s="26"/>
       <c r="C102" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B103" s="26"/>
       <c r="C103" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B104" s="26"/>
       <c r="C104" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B105" s="26"/>
       <c r="C105" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B106" s="26"/>
       <c r="C106" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B107" s="26"/>
       <c r="C107" s="10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B108" s="26"/>
       <c r="C108" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B109" s="26"/>
       <c r="C109" s="10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B110" s="26"/>
       <c r="C110" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B111" s="26"/>
       <c r="C111" s="10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B112" s="26"/>
       <c r="C112" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B113" s="26"/>
       <c r="C113" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B114" s="26"/>
       <c r="C114" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B115" s="26"/>
       <c r="C115" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B116" s="26"/>
       <c r="C116" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B117" s="26"/>
       <c r="C117" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B118" s="26"/>
       <c r="C118" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B119" s="26"/>
       <c r="C119" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B120" s="26"/>
       <c r="C120" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B121" s="26"/>
       <c r="C121" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B122" s="26"/>
       <c r="C122" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B123" s="26"/>
       <c r="C123" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B124" s="26"/>
       <c r="C124" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B125" s="26"/>
       <c r="C125" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B126" s="26"/>
       <c r="C126" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B127" s="26"/>
       <c r="C127" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B128" s="26"/>
       <c r="C128" s="10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B129" s="26"/>
       <c r="C129" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B130" s="26"/>
       <c r="C130" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B131" s="26"/>
       <c r="C131" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B132" s="26"/>
       <c r="C132" s="10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -4685,18 +4685,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
         <v>166</v>
-      </c>
-      <c r="B1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4706,22 +4706,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="52.5" customWidth="1"/>
+    <col min="2" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>30</v>
       </c>
@@ -4729,56 +4729,65 @@
         <v>31</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="G1" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" t="s">
+        <v>558</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -4803,10 +4812,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -4814,10 +4823,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
@@ -4825,10 +4834,10 @@
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -4836,10 +4845,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -4847,10 +4856,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -4858,10 +4867,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -4869,10 +4878,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -4880,10 +4889,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -4891,10 +4900,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -4902,7 +4911,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
@@ -4911,10 +4920,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>11</v>
@@ -4923,41 +4932,41 @@
         <v>2</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4993,8 +5002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7FA707-26D8-0546-9A99-D418F7F4E088}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5008,62 +5017,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>272</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5091,24 +5100,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>261</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5116,10 +5125,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5127,21 +5136,21 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5171,10 +5180,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>
@@ -5190,15 +5199,15 @@
       </c>
       <c r="G1" s="31"/>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>3</v>
@@ -5221,10 +5230,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>21</v>
@@ -5315,29 +5324,29 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -5358,7 +5367,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5369,7 +5378,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -5441,16 +5450,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>281</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5458,7 +5467,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5466,13 +5475,13 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5500,72 +5509,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -5592,72 +5601,72 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
         <v>76</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update activities and timelines
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/new_labels.xlsx
+++ b/tests/integration_test_files/new_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A035B35B-B4F9-0A49-B74C-519D951BB33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D3E3D6-3634-6240-AE50-74780BE4EEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66180" yWindow="7680" windowWidth="33600" windowHeight="19480" firstSheet="6" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="66180" yWindow="7680" windowWidth="33600" windowHeight="19480" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="565">
   <si>
     <t>Epoch</t>
   </si>
@@ -437,9 +437,6 @@
     <t>summaryMeasure</t>
   </si>
   <si>
-    <t>intercurrentEventName</t>
-  </si>
-  <si>
     <t>intercurrentEventStrategy</t>
   </si>
   <si>
@@ -461,9 +458,6 @@
     <t>Survival of all patients</t>
   </si>
   <si>
-    <t>intercurrentEventDescription</t>
-  </si>
-  <si>
     <t>IC Event Description</t>
   </si>
   <si>
@@ -843,12 +837,6 @@
   </si>
   <si>
     <t>Placebo Comparator Arm</t>
-  </si>
-  <si>
-    <t>activityName</t>
-  </si>
-  <si>
-    <t>activityDescription</t>
   </si>
   <si>
     <t>activityIsConditional</t>
@@ -1780,6 +1768,12 @@
   </si>
   <si>
     <t>TRT 2</t>
+  </si>
+  <si>
+    <t>ICE 1</t>
+  </si>
+  <si>
+    <t>ICE 2</t>
   </si>
 </sst>
 </file>
@@ -2337,10 +2331,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -2351,10 +2345,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -2365,10 +2359,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -2389,42 +2383,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="E9" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="F9" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="G9" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="H9" s="21" t="s">
         <v>147</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>153</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -2434,33 +2428,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>152</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="15">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2567,19 +2561,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>86</v>
@@ -2599,7 +2593,7 @@
         <v>89</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>90</v>
@@ -2622,7 +2616,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>94</v>
@@ -3002,23 +2996,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>107</v>
       </c>
@@ -3029,81 +3025,90 @@
         <v>69</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
         <v>131</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
         <v>135</v>
       </c>
-      <c r="C2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>563</v>
+      </c>
+      <c r="G2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
         <v>133</v>
       </c>
-      <c r="E2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
+      <c r="B5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
         <v>168</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>169</v>
       </c>
-      <c r="C5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>564</v>
+      </c>
+      <c r="G5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" t="s">
         <v>170</v>
-      </c>
-      <c r="E5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3135,62 +3140,62 @@
         <v>107</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>61</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>191</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="G3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3226,152 +3231,152 @@
         <v>107</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>61</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>58</v>
       </c>
       <c r="F1" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>196</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>204</v>
-      </c>
       <c r="F5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3385,7 +3390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3402,119 +3407,119 @@
         <v>107</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>61</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>230</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>231</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>565</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3541,16 +3546,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
@@ -3559,1212 +3564,1212 @@
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="10" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="10" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="10" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="10" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="10" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="10" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="10" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="10" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="10" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="10" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="10" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="10" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="10" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="10" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="10" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B44" s="26"/>
       <c r="C44" s="10" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="10" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="10" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="10" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="10" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B52" s="26"/>
       <c r="C52" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B55" s="26"/>
       <c r="C55" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B56" s="26"/>
       <c r="C56" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B57" s="26"/>
       <c r="C57" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B58" s="26"/>
       <c r="C58" s="10" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B59" s="26"/>
       <c r="C59" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B60" s="26"/>
       <c r="C60" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B61" s="26"/>
       <c r="C61" s="10" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B62" s="26"/>
       <c r="C62" s="10" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B63" s="26"/>
       <c r="C63" s="10" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B64" s="26"/>
       <c r="C64" s="10" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B65" s="26"/>
       <c r="C65" s="10" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B66" s="26"/>
       <c r="C66" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B67" s="26"/>
       <c r="C67" s="10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B68" s="26"/>
       <c r="C68" s="10" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B69" s="26"/>
       <c r="C69" s="10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B70" s="26"/>
       <c r="C70" s="10" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B71" s="26"/>
       <c r="C71" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B72" s="26"/>
       <c r="C72" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B73" s="26"/>
       <c r="C73" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B74" s="26"/>
       <c r="C74" s="10" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B75" s="26"/>
       <c r="C75" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B76" s="26"/>
       <c r="C76" s="10" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B77" s="26"/>
       <c r="C77" s="10" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B78" s="26"/>
       <c r="C78" s="10" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B79" s="26"/>
       <c r="C79" s="10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B80" s="26"/>
       <c r="C80" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B82" s="26"/>
       <c r="C82" s="10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B83" s="26"/>
       <c r="C83" s="10" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B84" s="26"/>
       <c r="C84" s="10" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B85" s="26"/>
       <c r="C85" s="10" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B86" s="26"/>
       <c r="C86" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B87" s="26"/>
       <c r="C87" s="10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B88" s="26"/>
       <c r="C88" s="10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="B89" s="26"/>
       <c r="C89" s="10" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B90" s="26"/>
       <c r="C90" s="10" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="10" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B92" s="26"/>
       <c r="C92" s="10" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B93" s="26"/>
       <c r="C93" s="10" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B94" s="26"/>
       <c r="C94" s="10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B95" s="26"/>
       <c r="C95" s="10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B96" s="26"/>
       <c r="C96" s="10" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B97" s="26"/>
       <c r="C97" s="10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B98" s="26"/>
       <c r="C98" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B99" s="26"/>
       <c r="C99" s="10" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B100" s="26"/>
       <c r="C100" s="10" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B101" s="26"/>
       <c r="C101" s="10" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B102" s="26"/>
       <c r="C102" s="10" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B103" s="26"/>
       <c r="C103" s="10" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B104" s="26"/>
       <c r="C104" s="10" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B105" s="26"/>
       <c r="C105" s="10" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B106" s="26"/>
       <c r="C106" s="10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B107" s="26"/>
       <c r="C107" s="10" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B108" s="26"/>
       <c r="C108" s="10" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B109" s="26"/>
       <c r="C109" s="10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B110" s="26"/>
       <c r="C110" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B111" s="26"/>
       <c r="C111" s="10" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B112" s="26"/>
       <c r="C112" s="10" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B113" s="26"/>
       <c r="C113" s="10" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B114" s="26"/>
       <c r="C114" s="10" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B115" s="26"/>
       <c r="C115" s="10" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B116" s="26"/>
       <c r="C116" s="10" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B117" s="26"/>
       <c r="C117" s="10" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B118" s="26"/>
       <c r="C118" s="10" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B119" s="26"/>
       <c r="C119" s="10" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B120" s="26"/>
       <c r="C120" s="10" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B121" s="26"/>
       <c r="C121" s="10" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B122" s="26"/>
       <c r="C122" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B123" s="26"/>
       <c r="C123" s="10" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B124" s="26"/>
       <c r="C124" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B125" s="26"/>
       <c r="C125" s="10" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B126" s="26"/>
       <c r="C126" s="10" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B127" s="26"/>
       <c r="C127" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B128" s="26"/>
       <c r="C128" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B129" s="26"/>
       <c r="C129" s="10" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B130" s="26"/>
       <c r="C130" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B131" s="26"/>
       <c r="C131" s="10" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B132" s="26"/>
       <c r="C132" s="10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -4788,18 +4793,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
         <v>163</v>
-      </c>
-      <c r="B1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4832,10 +4837,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>58</v>
@@ -4858,10 +4863,10 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -4881,10 +4886,10 @@
         <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F3" t="s">
         <v>52</v>
@@ -4915,10 +4920,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -4929,7 +4934,7 @@
         <v>61</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
@@ -4937,10 +4942,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>541</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>545</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -4951,7 +4956,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -4962,7 +4967,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -4973,7 +4978,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4984,7 +4989,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -4995,7 +5000,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -5006,7 +5011,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -5014,10 +5019,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
@@ -5025,7 +5030,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -5034,7 +5039,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>40</v>
@@ -5054,16 +5059,16 @@
         <v>38</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5071,16 +5076,16 @@
         <v>39</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5132,22 +5137,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>61</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>256</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5155,19 +5160,19 @@
         <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5181,13 +5186,13 @@
         <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5216,13 +5221,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>61</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D1" s="24" t="s">
         <v>58</v>
@@ -5233,13 +5238,13 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5247,13 +5252,13 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5261,13 +5266,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5275,13 +5280,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -5293,7 +5298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -5311,10 +5316,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>
@@ -5335,10 +5340,10 @@
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>3</v>
@@ -5361,10 +5366,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>21</v>
@@ -5455,29 +5460,29 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -5498,7 +5503,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5564,60 +5569,70 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8389B3-D1BB-1047-BA06-7E793B938DBA}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="24" style="7" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="2" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="24" style="7" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>264</v>
+        <v>465</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5738,7 +5753,7 @@
         <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>71</v>
@@ -5757,13 +5772,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B2" t="s">
         <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -5780,13 +5795,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -5803,13 +5818,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B4" t="s">
         <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D4">
         <v>20</v>

</xml_diff>